<commit_message>
finalized spice scheme, digikey bom, total bom
</commit_message>
<xml_diff>
--- a/Total Used Materials.xlsx
+++ b/Total Used Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\home\Desktop\ECE 411\Synthy Repo\synthy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ACEA08-C058-453B-817F-9BAD20A46DF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9BB5B1-CFE4-4842-9322-D415F42BA2FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="18720" windowHeight="11949" xr2:uid="{6BA9F994-4B08-4D4A-8C9A-5F972169FB34}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="90">
   <si>
     <t>SOURCE</t>
   </si>
@@ -177,12 +177,6 @@
     <t>500k Log Potentiometer</t>
   </si>
   <si>
-    <t># to Order</t>
-  </si>
-  <si>
-    <t>Quantity in Package</t>
-  </si>
-  <si>
     <t>490-2876-ND</t>
   </si>
   <si>
@@ -295,6 +289,18 @@
   </si>
   <si>
     <t>399-1168-1-ND</t>
+  </si>
+  <si>
+    <t>493-14498-ND</t>
+  </si>
+  <si>
+    <t>10u electrolytic capacitor</t>
+  </si>
+  <si>
+    <t>Quantity Priced</t>
+  </si>
+  <si>
+    <t>Quantity to Order</t>
   </si>
 </sst>
 </file>
@@ -675,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BCB7EE-4B0C-4B2B-B82C-E6755F966470}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -687,6 +693,7 @@
     <col min="3" max="3" width="17.69140625" customWidth="1"/>
     <col min="4" max="4" width="21.07421875" customWidth="1"/>
     <col min="5" max="5" width="13.69140625" customWidth="1"/>
+    <col min="6" max="6" width="19.84375" customWidth="1"/>
     <col min="7" max="8" width="14.07421875" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="16.3046875" customWidth="1"/>
@@ -710,13 +717,13 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -1112,7 +1119,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
         <v>30</v>
@@ -1130,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="H19">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J19" t="s">
         <v>28</v>
@@ -1141,7 +1148,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="D20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J20" t="s">
         <v>28</v>
@@ -1175,13 +1182,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B22" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E22">
         <v>1.5</v>
@@ -1201,13 +1208,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B23" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E23">
         <v>1.5</v>
@@ -1227,13 +1234,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B24" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
         <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E24">
         <v>0.32</v>
@@ -1253,13 +1260,13 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E25">
         <v>0.56000000000000005</v>
@@ -1279,13 +1286,13 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B26" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E26">
         <v>0.95</v>
@@ -1305,13 +1312,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
         <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E27">
         <v>0.49</v>
@@ -1325,16 +1332,19 @@
       <c r="H27">
         <v>4</v>
       </c>
+      <c r="J27" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B28" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
         <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E28">
         <v>0.66</v>
@@ -1348,19 +1358,22 @@
       <c r="H28">
         <v>10</v>
       </c>
+      <c r="J28" t="s">
+        <v>28</v>
+      </c>
       <c r="K28" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E29">
         <v>0.46</v>
@@ -1372,21 +1385,24 @@
         <v>3</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="J29" t="s">
+        <v>28</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B30" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E30">
         <v>0.35</v>
@@ -1398,21 +1414,24 @@
         <v>2</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="J30" t="s">
+        <v>28</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B31" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E31">
         <v>0.26</v>
@@ -1426,19 +1445,22 @@
       <c r="H31">
         <v>5</v>
       </c>
+      <c r="J31" t="s">
+        <v>28</v>
+      </c>
       <c r="K31" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B32" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E32">
         <v>8.07</v>
@@ -1449,19 +1471,25 @@
       <c r="G32">
         <v>4</v>
       </c>
+      <c r="H32">
+        <v>50</v>
+      </c>
+      <c r="J32" t="s">
+        <v>28</v>
+      </c>
       <c r="K32" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B33" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E33">
         <v>3.06</v>
@@ -1473,21 +1501,24 @@
         <v>2</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="J33" t="s">
+        <v>28</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B34" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E34">
         <v>1.67</v>
@@ -1499,21 +1530,24 @@
         <v>1</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="J34" t="s">
+        <v>28</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B35" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E35">
         <v>3.06</v>
@@ -1527,19 +1561,22 @@
       <c r="H35">
         <v>1</v>
       </c>
+      <c r="J35" t="s">
+        <v>28</v>
+      </c>
       <c r="K35" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B36" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E36">
         <v>1.96</v>
@@ -1553,16 +1590,19 @@
       <c r="H36">
         <v>2</v>
       </c>
+      <c r="J36" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B37" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E37">
         <v>4.54</v>
@@ -1571,21 +1611,24 @@
         <v>10</v>
       </c>
       <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
         <v>2</v>
       </c>
-      <c r="H37">
-        <v>1</v>
+      <c r="J37" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B38" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E38">
         <v>1.37</v>
@@ -1594,10 +1637,39 @@
         <v>10</v>
       </c>
       <c r="G38">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H38">
         <v>5</v>
+      </c>
+      <c r="J38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39">
+        <v>3.98</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="J39" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to reflect currently purchased items
</commit_message>
<xml_diff>
--- a/Total Used Materials.xlsx
+++ b/Total Used Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\home\Desktop\ECE 411\Synthy Repo\synthy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9BB5B1-CFE4-4842-9322-D415F42BA2FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C48E96-8944-4C50-8204-39D15E24232A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="18720" windowHeight="11949" xr2:uid="{6BA9F994-4B08-4D4A-8C9A-5F972169FB34}"/>
   </bookViews>
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BCB7EE-4B0C-4B2B-B82C-E6755F966470}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -761,7 +761,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
@@ -787,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
@@ -813,7 +813,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
@@ -839,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
@@ -917,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
@@ -1027,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">

</xml_diff>